<commit_message>
Formatacao da impressao da matriz confusao
</commit_message>
<xml_diff>
--- a/trabalho/vetores_caracteristicas/Imagens Seg1 benign.xlsx
+++ b/trabalho/vetores_caracteristicas/Imagens Seg1 benign.xlsx
@@ -346,13 +346,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2.7146045689148273</v>
+        <v>2.6803049333392641</v>
       </c>
       <c r="B1">
-        <v>3.5604435535863543</v>
+        <v>4.1574160576240322</v>
       </c>
       <c r="C1">
-        <v>133480</v>
+        <v>132758</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -379,13 +379,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2.6850329762824661</v>
+        <v>2.6314883984528774</v>
       </c>
       <c r="B4">
-        <v>2.8815188429407783</v>
+        <v>4.3197514589307975</v>
       </c>
       <c r="C4">
-        <v>200615</v>
+        <v>221868</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>